<commit_message>
Update uhq rates to reflect equations in paper (lines 58-63)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -530,22 +530,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6747343356739812</v>
+        <v>0.6610309099806798</v>
       </c>
       <c r="C3" t="n">
         <v>0.1188067775532411</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0.0001083189802580445</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0107235790455464</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.061961759676667e-06</v>
+      </c>
       <c r="G3" t="n">
-        <v>0.001805597802994974</v>
+        <v>0.0004024156795688895</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08755813721922846</v>
+        <v>2.331262728070345e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>0.003145332693166995</v>
+        <v>0.002716118733894493</v>
       </c>
       <c r="J3" t="n">
         <v>0.1180921373645059</v>
@@ -559,24 +565,32 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.639699954125287</v>
+        <v>0.6033558379651277</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1421385171951744</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+        <v>0.1429607227367725</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0002478541818747085</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01411739725565055</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.294531820301569e-06</v>
+      </c>
       <c r="G4" t="n">
-        <v>0.002411164148442924</v>
+        <v>0.0005370910581833254</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2003490836037339</v>
+        <v>5.295560199292023e-05</v>
       </c>
       <c r="I4" t="n">
-        <v>0.003655732507968392</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>0.003078316154487901</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1180958239391973</v>
+      </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
@@ -586,24 +600,32 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5996392474775651</v>
+        <v>0.5359785339991505</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1616033934072441</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+        <v>0.1644335827547162</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0004124671320663437</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.01699094641782112</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.546751745248789e-05</v>
+      </c>
       <c r="G5" t="n">
-        <v>0.00288954692838328</v>
+        <v>0.0006473095863210778</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3326136709421486</v>
+        <v>8.792782943499545e-05</v>
       </c>
       <c r="I5" t="n">
-        <v>0.004370537331837111</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+        <v>0.003698622445585419</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1181042489748803</v>
+      </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
@@ -613,24 +635,32 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.557298308147462</v>
+        <v>0.4650191159006192</v>
       </c>
       <c r="C6" t="n">
-        <v>0.178105041358886</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+        <v>0.1841531339022194</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0005982383516741455</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.01954671242480341</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.243393818778045e-05</v>
+      </c>
       <c r="G6" t="n">
-        <v>0.003288125078555519</v>
+        <v>0.0007451094171468894</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4800557797607952</v>
+        <v>0.0001273964138132682</v>
       </c>
       <c r="I6" t="n">
-        <v>0.004975284438573783</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+        <v>0.004258755709809346</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1181182641307136</v>
+      </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
@@ -640,24 +670,32 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5147450249171091</v>
+        <v>0.3950488935544532</v>
       </c>
       <c r="C7" t="n">
-        <v>0.192227369059824</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+        <v>0.2025092421498664</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0008024714385099327</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.02189480104361739</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.009267894412248e-05</v>
+      </c>
       <c r="G7" t="n">
-        <v>0.003625890453701698</v>
+        <v>0.000834857334227037</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6393761080456123</v>
+        <v>0.0001707883633715627</v>
       </c>
       <c r="I7" t="n">
-        <v>0.005487932017929077</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>0.004772875656516981</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1181385879582081</v>
+      </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
@@ -667,24 +705,32 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4734315958853085</v>
+        <v>0.3292647662262045</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2043342595651563</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+        <v>0.2195514028011575</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001023013328811494</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.02408144988626477</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.836299983043104e-05</v>
+      </c>
       <c r="G8" t="n">
-        <v>0.003914889655998293</v>
+        <v>0.0009183749060616591</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8079341250083645</v>
+        <v>0.0002176461459453748</v>
       </c>
       <c r="I8" t="n">
-        <v>0.005926519893516458</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
+        <v>0.005251236499678021</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1181658474375374</v>
+      </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
@@ -694,24 +740,32 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4342993372653224</v>
+        <v>0.2697048107417248</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2146474624847384</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+        <v>0.2351391741760236</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.001257830638966161</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.02611247634064593</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.716864896123105e-05</v>
+      </c>
       <c r="G9" t="n">
-        <v>0.004162634050629493</v>
+        <v>0.0009959179726567527</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9835162012863319</v>
+        <v>0.0002675376615731995</v>
       </c>
       <c r="I9" t="n">
-        <v>0.006302489515856018</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
+        <v>0.00569538614585585</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.1182005964295872</v>
+      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -721,24 +775,32 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3978930522944134</v>
+        <v>0.2174595847269764</v>
       </c>
       <c r="C10" t="n">
-        <v>0.223303819972321</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+        <v>0.2490511482660261</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.001504778390086337</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02797113676370552</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5.642918962823764e-05</v>
+      </c>
       <c r="G10" t="n">
-        <v>0.00437370435027698</v>
+        <v>0.001066865829623726</v>
       </c>
       <c r="H10" t="n">
-        <v>1.164185786260511</v>
+        <v>0.000320007096464036</v>
       </c>
       <c r="I10" t="n">
-        <v>0.006622826319453562</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>0.006101824188918121</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.1182433197403573</v>
+      </c>
       <c r="K10" t="n">
         <v>0</v>
       </c>
@@ -748,24 +810,32 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3644665278965953</v>
+        <v>0.1728730253175389</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2303948923234032</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+        <v>0.2610600687904289</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.001761505973083151</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.02963106546515542</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6.605647399061816e-05</v>
+      </c>
       <c r="G11" t="n">
-        <v>0.004550926263841794</v>
+        <v>0.001130220062619847</v>
       </c>
       <c r="H11" t="n">
-        <v>1.348193289618368</v>
+        <v>0.0003745549405708796</v>
       </c>
       <c r="I11" t="n">
-        <v>0.006891838845065729</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>0.006464859321873347</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.1182944293311354</v>
+      </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
@@ -775,24 +845,32 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3340709293331141</v>
+        <v>0.1357337436702637</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2359926965648763</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+        <v>0.270980849234879</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.002025455888385338</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.03106519599611967</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.595459581445016e-05</v>
+      </c>
       <c r="G12" t="n">
-        <v>0.004696185815986595</v>
+        <v>0.001184948875676186</v>
       </c>
       <c r="H12" t="n">
-        <v>1.533926923062755</v>
+        <v>0.0004306377197764544</v>
       </c>
       <c r="I12" t="n">
-        <v>0.007112399280093508</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>0.006778588842880892</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.1183542573351966</v>
+      </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
@@ -802,24 +880,32 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3066241672099865</v>
+        <v>0.1054532548958411</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2401651437985383</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+        <v>0.2786970820657173</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.002293920142592403</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.03225146565545564</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8.602200534721511e-05</v>
+      </c>
       <c r="G13" t="n">
-        <v>0.004810959936127666</v>
+        <v>0.001230207691529504</v>
       </c>
       <c r="H13" t="n">
-        <v>1.719889884884927</v>
+        <v>0.0004876799801776078</v>
       </c>
       <c r="I13" t="n">
-        <v>0.007286751715997009</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
+        <v>0.007038168474262355</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.1184230490317034</v>
+      </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
@@ -829,24 +915,32 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2819626655511144</v>
+        <v>0.08122352199166959</v>
       </c>
       <c r="C14" t="n">
-        <v>0.242984248571435</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+        <v>0.284170907685431</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.002564126877078677</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.03317596642555665</v>
+      </c>
+      <c r="F14" t="n">
+        <v>9.615475789045036e-05</v>
+      </c>
       <c r="G14" t="n">
-        <v>0.004896635498731643</v>
+        <v>0.001265461529818443</v>
       </c>
       <c r="H14" t="n">
-        <v>1.904693157592732</v>
+        <v>0.0005450926966593927</v>
       </c>
       <c r="I14" t="n">
-        <v>0.007416998788891662</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
+        <v>0.007240518539350068</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.1185009577348645</v>
+      </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
@@ -856,24 +950,32 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2598783814304141</v>
+        <v>0.06214598912384005</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2445295451473689</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+        <v>0.2874407401606637</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.002833336413742991</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0338341199251522</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0001062501155153621</v>
+      </c>
       <c r="G15" t="n">
-        <v>0.004954679700104095</v>
+        <v>0.001290531347417073</v>
       </c>
       <c r="H15" t="n">
-        <v>2.087056470294427</v>
+        <v>0.0006022936826127146</v>
       </c>
       <c r="I15" t="n">
-        <v>0.007505362121899797</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+        <v>0.007384593654013793</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1185880426250438</v>
+      </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
@@ -883,24 +985,32 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2401442290844708</v>
+        <v>0.04732759066751309</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2448885282524558</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+        <v>0.2886110216189984</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.003098931882350984</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.03423041002072676</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0001162099455881619</v>
+      </c>
       <c r="G16" t="n">
-        <v>0.004986711689129398</v>
+        <v>0.001305584805555648</v>
       </c>
       <c r="H16" t="n">
-        <v>2.265812547919131</v>
+        <v>0.0006587268482405278</v>
       </c>
       <c r="I16" t="n">
-        <v>0.007554292392168352</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
+        <v>0.007471333160687757</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.1186842698416305</v>
+      </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
@@ -910,24 +1020,32 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2225308010234213</v>
+        <v>0.03594391918243994</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2441554081399047</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+        <v>0.2878376812170164</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.003358495015587955</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.03437716828611342</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0001259435630845483</v>
+      </c>
       <c r="G17" t="n">
-        <v>0.004994512771818227</v>
+        <v>0.001311090446540417</v>
       </c>
       <c r="H17" t="n">
-        <v>2.439911668982278</v>
+        <v>0.0007138783070026377</v>
       </c>
       <c r="I17" t="n">
-        <v>0.007566485756185774</v>
-      </c>
-      <c r="J17" t="inlineStr"/>
+        <v>0.007503401035747628</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.1187895166536603</v>
+      </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
@@ -937,24 +1055,32 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2068167950119663</v>
+        <v>0.02727379174787814</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2424290521803803</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+        <v>0.2853122633939841</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.003609862372611912</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.03429284873353516</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0001353698389729467</v>
+      </c>
       <c r="G18" t="n">
-        <v>0.004980001710571369</v>
+        <v>0.001307752024484692</v>
       </c>
       <c r="H18" t="n">
-        <v>2.608424888146481</v>
+        <v>0.000767288323116903</v>
       </c>
       <c r="I18" t="n">
-        <v>0.007544846979702148</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
+        <v>0.007484811232463836</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1189035782044729</v>
+      </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
@@ -964,24 +1090,32 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1927950345484489</v>
+        <v>0.02071178317371192</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2398106726597841</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+        <v>0.2812468518289091</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003851160942251559</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.03400014388624832</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0001444185353344334</v>
+      </c>
       <c r="G19" t="n">
-        <v>0.00494519307679269</v>
+        <v>0.001296436522695202</v>
       </c>
       <c r="H19" t="n">
-        <v>2.770545171893349</v>
+        <v>0.0008185588772350957</v>
       </c>
       <c r="I19" t="n">
-        <v>0.007492426612520741</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
+        <v>0.007420516096245826</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.1190261761657504</v>
+      </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
@@ -991,24 +1125,32 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1802754998242862</v>
+        <v>0.01576579506419083</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2364015969967007</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+        <v>0.275861086836404</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.004080824658063207</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.03352419478069391</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0001530309246773702</v>
+      </c>
       <c r="G20" t="n">
-        <v>0.00489215019888546</v>
+        <v>0.001278105593438077</v>
       </c>
       <c r="H20" t="n">
-        <v>2.925586259560325</v>
+        <v>0.0008673571758888849</v>
       </c>
       <c r="I20" t="n">
-        <v>0.007412349794217876</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
+        <v>0.007316013792821563</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1191569686006572</v>
+      </c>
       <c r="K20" t="n">
         <v>0</v>
       </c>
@@ -1018,24 +1160,32 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1690863982640558</v>
+        <v>0.01204590676195057</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2323013032523766</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+        <v>0.269371870112436</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.004297594871841122</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.03289104911371443</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.000161159807694042</v>
+      </c>
       <c r="G21" t="n">
-        <v>0.004822939653792392</v>
+        <v>0.001253756390368878</v>
       </c>
       <c r="H21" t="n">
-        <v>3.072979393379436</v>
+        <v>0.0009134157521072791</v>
       </c>
       <c r="I21" t="n">
-        <v>0.007307747288912762</v>
-      </c>
-      <c r="J21" t="inlineStr"/>
+        <v>0.007177009138556126</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.1192955603878405</v>
+      </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
@@ -1045,24 +1195,32 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1590740017305506</v>
+        <v>0.00924928192884648</v>
       </c>
       <c r="C22" t="n">
-        <v>0.227605802915004</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+        <v>0.2619858324171081</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.004500508459564494</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.03212643818012798</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0001687690672336685</v>
+      </c>
       <c r="G22" t="n">
-        <v>0.004739591094331103</v>
+        <v>0.001224374555324059</v>
       </c>
       <c r="H22" t="n">
-        <v>3.212268234519617</v>
+        <v>0.0009565299379269465</v>
       </c>
       <c r="I22" t="n">
-        <v>0.007181694543678657</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
+        <v>0.007009143826920431</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.11944151366151</v>
+      </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
switched the death & recovery rates in initial data, added exposed/recovered/sum columns, created record of data sources
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,49 +446,64 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>exposed</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>infected</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>UD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>UR</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>HD</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>HR</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>QD</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>QR</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>died</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>recovered</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>immune state</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -498,31 +513,40 @@
         <v>0.7013472200632157</v>
       </c>
       <c r="C2" t="n">
+        <v>0.7013472200632157</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.09026581688170371</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
       <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.07522151406808643</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>1.450852375770765e-05</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>3.033374237335405e-07</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.01502949095243584</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
+        <v>2.901704751541531e-05</v>
+      </c>
+      <c r="L2" t="n">
         <v>0.1180921291258615</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.701347220063216</v>
       </c>
     </row>
     <row r="3">
@@ -533,31 +557,40 @@
         <v>0.6610309099806798</v>
       </c>
       <c r="C3" t="n">
+        <v>0.6995826969419586</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.1188067775532411</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.0001083189802580445</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.0107235790455464</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>4.061961759676667e-06</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.0004024156795688895</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>2.331262728070345e-05</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.002716118733894493</v>
       </c>
-      <c r="J3" t="n">
-        <v>0.1180921373645059</v>
-      </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>2.902528615984391e-05</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0004112392469746046</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.493838456037322</v>
       </c>
     </row>
     <row r="4">
@@ -568,31 +601,40 @@
         <v>0.6033558379651277</v>
       </c>
       <c r="C4" t="n">
+        <v>0.7152828071409932</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.1429607227367725</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.0002478541818747085</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.01411739725565055</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>9.294531820301569e-06</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.0005370910581833254</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>5.295560199292023e-05</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.003078316154487901</v>
       </c>
-      <c r="J4" t="n">
-        <v>0.1180958239391973</v>
-      </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>3.271186085128183e-05</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0005266132234678202</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.480201601711222</v>
       </c>
     </row>
     <row r="5">
@@ -603,31 +645,40 @@
         <v>0.5359785339991505</v>
       </c>
       <c r="C5" t="n">
+        <v>0.7397431426785109</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.1644335827547162</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.0004124671320663437</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.01699094641782112</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1.546751745248789e-05</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.0006473095863210778</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>8.792782943499545e-05</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.003698622445585419</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.1181042489748803</v>
-      </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>4.11368965342757e-05</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.0006336332576286177</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.462682770515222</v>
       </c>
     </row>
     <row r="6">
@@ -638,31 +689,40 @@
         <v>0.4650191159006192</v>
       </c>
       <c r="C6" t="n">
+        <v>0.7663179722163316</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.1841531339022194</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.0005982383516741455</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.01954671242480341</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>2.243393818778045e-05</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.0007451094171468894</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>0.0001273964138132682</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.004258755709809346</v>
       </c>
-      <c r="J6" t="n">
-        <v>0.1181182641307136</v>
-      </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>5.515205236754834e-05</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.0007290662323813206</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.441573086559354</v>
       </c>
     </row>
     <row r="7">
@@ -673,31 +733,40 @@
         <v>0.3950488935544532</v>
       </c>
       <c r="C7" t="n">
+        <v>0.7903091162295177</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.2025092421498664</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.0008024714385099327</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.02189480104361739</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>3.009267894412248e-05</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.000834857334227037</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.0001707883633715627</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.004772875656516981</v>
       </c>
-      <c r="J7" t="n">
-        <v>0.1181385879582081</v>
-      </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>7.547587986205919e-05</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0008167274476885717</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.417265341776575</v>
       </c>
     </row>
     <row r="8">
@@ -708,31 +777,40 @@
         <v>0.3292647662262045</v>
       </c>
       <c r="C8" t="n">
+        <v>0.8086746965839954</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.2195514028011575</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>0.001023013328811494</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.02408144988626477</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>3.836299983043104e-05</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>0.0009183749060616591</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>0.0002176461459453748</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.005251236499678021</v>
       </c>
-      <c r="J8" t="n">
-        <v>0.1181658474375374</v>
-      </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>0.0001027353591913873</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0008983480896995168</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.39002203282684</v>
       </c>
     </row>
     <row r="9">
@@ -743,31 +821,40 @@
         <v>0.2697048107417248</v>
       </c>
       <c r="C9" t="n">
+        <v>0.8197141702734354</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.2351391741760236</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.001257830638966161</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.02611247634064593</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>4.716864896123105e-05</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.0009959179726567527</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.0002675376615731995</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>0.00569538614585585</v>
       </c>
-      <c r="J9" t="n">
-        <v>0.1182005964295872</v>
-      </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>0.0001374843512411309</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0009741542340481884</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.360046111185132</v>
       </c>
     </row>
     <row r="10">
@@ -778,31 +865,40 @@
         <v>0.2174595847269764</v>
       </c>
       <c r="C10" t="n">
+        <v>0.8227765460717776</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.2490511482660261</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.001504778390086337</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.02797113676370552</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>5.642918962823764e-05</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.001066865829623726</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>0.000320007096464036</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.006101824188918121</v>
       </c>
-      <c r="J10" t="n">
-        <v>0.1182433197403573</v>
-      </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.0001802076620112761</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.001043526145171184</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.327532054330388</v>
       </c>
     </row>
     <row r="11">
@@ -813,31 +909,40 @@
         <v>0.1728730253175389</v>
       </c>
       <c r="C11" t="n">
+        <v>0.8179965127169085</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.2610600687904289</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.001761505973083151</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.02963106546515542</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>6.605647399061816e-05</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.001130220062619847</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0.0003745549405708796</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>0.006464859321873347</v>
       </c>
-      <c r="J11" t="n">
-        <v>0.1182944293311354</v>
-      </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.0002313172527893831</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.00110548214486326</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.292694668459822</v>
       </c>
     </row>
     <row r="12">
@@ -848,31 +953,40 @@
         <v>0.1357337436702637</v>
       </c>
       <c r="C12" t="n">
+        <v>0.8060560036011692</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.270980849234879</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.002025455888385338</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.03106519599611967</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>7.595459581445016e-05</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>0.001184948875676186</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>0.0004306377197764544</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.006778588842880892</v>
       </c>
-      <c r="J12" t="n">
-        <v>0.1183542573351966</v>
-      </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>0.0002911452568505292</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.00115901252268354</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.255781536204499</v>
       </c>
     </row>
     <row r="13">
@@ -883,31 +997,40 @@
         <v>0.1054532548958411</v>
       </c>
       <c r="C13" t="n">
+        <v>0.7879731321595217</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.2786970820657173</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.002293920142592403</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>0.03225146565545564</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>8.602200534721511e-05</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.001230207691529504</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.0004876799801776078</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.007038168474262355</v>
       </c>
-      <c r="J13" t="n">
-        <v>0.1184230490317034</v>
-      </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>0.000359936953357352</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.00120329317772213</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.217074163201525</v>
       </c>
     </row>
     <row r="14">
@@ -918,31 +1041,40 @@
         <v>0.08122352199166959</v>
       </c>
       <c r="C14" t="n">
+        <v>0.7649244771341219</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.284170907685431</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>0.002564126877078677</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>0.03317596642555665</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>9.615475789045036e-05</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>0.001265461529818443</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>0.0005450926966593927</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.007240518539350068</v>
       </c>
-      <c r="J14" t="n">
-        <v>0.1185009577348645</v>
-      </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>0.0004378456565185131</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.00123780377954357</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1.176881877073638</v>
       </c>
     </row>
     <row r="15">
@@ -953,31 +1085,40 @@
         <v>0.06214598912384005</v>
       </c>
       <c r="C15" t="n">
+        <v>0.7381065413739042</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.2874407401606637</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>0.002833336413742991</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>0.0338341199251522</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.0001062501155153621</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>0.001290531347417073</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>0.0006022936826127146</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.007384593654013793</v>
       </c>
-      <c r="J15" t="n">
-        <v>0.1185880426250438</v>
-      </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.000524930546697753</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.001262372034323321</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1.135531698377883</v>
       </c>
     </row>
     <row r="16">
@@ -988,31 +1129,40 @@
         <v>0.04732759066751309</v>
       </c>
       <c r="C16" t="n">
+        <v>0.7086385473477969</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.2886110216189984</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>0.003098931882350984</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0.03423041002072676</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>0.0001162099455881619</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>0.001305584805555648</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>0.0006587268482405278</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.007471333160687757</v>
       </c>
-      <c r="J16" t="n">
-        <v>0.1186842698416305</v>
-      </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>0.0006211577632845155</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.001277163991553548</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1.093356678052296</v>
       </c>
     </row>
     <row r="17">
@@ -1023,31 +1173,40 @@
         <v>0.03594391918243994</v>
       </c>
       <c r="C17" t="n">
+        <v>0.6775039059920022</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.2878376812170164</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>0.003358495015587955</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.03437716828611342</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>0.0001259435630845483</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.001311090446540417</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.0007138783070026377</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.007503401035747628</v>
       </c>
-      <c r="J17" t="n">
-        <v>0.1187895166536603</v>
-      </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>0.0007264045753143201</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.00128263888858664</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.050684526509436</v>
       </c>
     </row>
     <row r="18">
@@ -1058,31 +1217,40 @@
         <v>0.02727379174787814</v>
       </c>
       <c r="C18" t="n">
+        <v>0.6455237990670438</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.2853122633939841</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>0.003609862372611912</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.03429284873353516</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>0.0001353698389729467</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0.001307752024484692</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>0.000767288323116903</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.007484811232463836</v>
       </c>
-      <c r="J18" t="n">
-        <v>0.1189035782044729</v>
-      </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>0.0008404661261269205</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.001279484839469663</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.007827737699688</v>
       </c>
     </row>
     <row r="19">
@@ -1093,31 +1261,40 @@
         <v>0.02071178317371192</v>
       </c>
       <c r="C19" t="n">
+        <v>0.6133543796971874</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.2812468518289091</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0.003851160942251559</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.03400014388624832</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>0.0001444185353344334</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.001296436522695202</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>0.0008185588772350957</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>0.007420516096245826</v>
       </c>
-      <c r="J19" t="n">
-        <v>0.1190261761657504</v>
-      </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>0.0009630640874043328</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.001268548529928728</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.9650758621771519</v>
       </c>
     </row>
     <row r="20">
@@ -1128,31 +1305,40 @@
         <v>0.01576579506419083</v>
       </c>
       <c r="C20" t="n">
+        <v>0.5814991050248772</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.275861086836404</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>0.004080824658063207</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.03352419478069391</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>0.0001530309246773702</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>0.001278105593438077</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>0.0008673571758888849</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.007316013792821563</v>
       </c>
-      <c r="J20" t="n">
-        <v>0.1191569686006572</v>
-      </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>0.001093856522311167</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.001250768369074226</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.9226901387424405</v>
       </c>
     </row>
     <row r="21">
@@ -1163,31 +1349,40 @@
         <v>0.01204590676195057</v>
       </c>
       <c r="C21" t="n">
+        <v>0.5503290470256248</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.269371870112436</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>0.004297594871841122</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.03289104911371443</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.000161159807694042</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>0.001253756390368878</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>0.0009134157521072791</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>0.007177009138556126</v>
       </c>
-      <c r="J21" t="n">
-        <v>0.1192955603878405</v>
-      </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>0.001232448309494453</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.001227116875375494</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.8809003741591631</v>
       </c>
     </row>
     <row r="22">
@@ -1198,31 +1393,40 @@
         <v>0.00924928192884648</v>
       </c>
       <c r="C22" t="n">
+        <v>0.5201059290371914</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.2619858324171081</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>0.004500508459564494</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0.03212643818012798</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>0.0001687690672336685</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>0.001224374555324059</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>0.0009565299379269465</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.007009143826920431</v>
       </c>
-      <c r="J22" t="n">
-        <v>0.11944151366151</v>
-      </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>0.001378401583164016</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.001198554951317933</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.8399037639447255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated alpha equation to take in start and end week as input, initial implementation of vax strats
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -510,43 +510,43 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7013472200632157</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7013472200632157</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09026581688170371</v>
+        <v>0.01289511287924234</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.07522151406808643</v>
+        <v>0.01074592739936861</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1.450852375770765e-05</v>
+        <v>2.072645637406635e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>3.033374237335405e-07</v>
+        <v>4.333390484538357e-08</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01502949095243584</v>
+        <v>0.00214706950033147</v>
       </c>
       <c r="K2" t="n">
-        <v>2.901704751541531e-05</v>
+        <v>4.14529127481327e-06</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1180921291258615</v>
+        <v>0.0168702991656713</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1.701347220063216</v>
+        <v>0.2430495309010738</v>
       </c>
     </row>
     <row r="3">
@@ -554,43 +554,43 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6610309099806798</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6995826969419586</v>
+        <v>0.09418088452225222</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1188067775532411</v>
+        <v>0.01697239176792528</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0001083189802580445</v>
+        <v>1.54741354550908e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0107235790455464</v>
+        <v>0.001531939410053989</v>
       </c>
       <c r="G3" t="n">
-        <v>4.061961759676667e-06</v>
+        <v>5.802800795659052e-07</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0004024156795688895</v>
+        <v>5.748793720239029e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>2.331262728070345e-05</v>
+        <v>3.330374339716509e-06</v>
       </c>
       <c r="J3" t="n">
-        <v>0.002716118733894493</v>
+        <v>0.0003880168470961185</v>
       </c>
       <c r="K3" t="n">
-        <v>2.902528615984391e-05</v>
+        <v>4.14646822366887e-06</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0004112392469746046</v>
+        <v>5.874844645855104e-05</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>1.493838456037322</v>
+        <v>0.2134054305319081</v>
       </c>
     </row>
     <row r="4">
@@ -598,43 +598,43 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6033558379651277</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7152828071409932</v>
+        <v>0.08853003145091709</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1429607227367725</v>
+        <v>0.02007738607407162</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0002478541818747085</v>
+        <v>3.54077297838586e-05</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01411739725565055</v>
+        <v>0.002016770439371266</v>
       </c>
       <c r="G4" t="n">
-        <v>9.294531820301569e-06</v>
+        <v>1.327789866894697e-06</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0005370910581833254</v>
+        <v>7.672727130783347e-05</v>
       </c>
       <c r="I4" t="n">
-        <v>5.295560199292023e-05</v>
+        <v>7.565083759025392e-06</v>
       </c>
       <c r="J4" t="n">
-        <v>0.003078316154487901</v>
+        <v>0.0004397593204317707</v>
       </c>
       <c r="K4" t="n">
-        <v>3.271186085128183e-05</v>
+        <v>4.673121595079125e-06</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0005266132234678202</v>
+        <v>7.523043822024778e-05</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>1.480201601711222</v>
+        <v>0.2114573090621462</v>
       </c>
     </row>
     <row r="5">
@@ -642,43 +642,43 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5359785339991505</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7397431426785109</v>
+        <v>0.08321822956386206</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1644335827547162</v>
+        <v>0.0223775800500159</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0004124671320663437</v>
+        <v>5.85091766387965e-05</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01699094641782112</v>
+        <v>0.002386223830536418</v>
       </c>
       <c r="G5" t="n">
-        <v>1.546751745248789e-05</v>
+        <v>2.194094123954869e-06</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0006473095863210778</v>
+        <v>9.093326402336103e-05</v>
       </c>
       <c r="I5" t="n">
-        <v>8.792782943499545e-05</v>
+        <v>1.247299486266094e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>0.003698622445585419</v>
+        <v>0.0005196506076645026</v>
       </c>
       <c r="K5" t="n">
-        <v>4.11368965342757e-05</v>
+        <v>5.876697764851445e-06</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0006336332576286177</v>
+        <v>8.899489842649483e-05</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>1.462682770515222</v>
+        <v>0.2089530955207405</v>
       </c>
     </row>
     <row r="6">
@@ -686,43 +686,43 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4650191159006192</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7663179722163316</v>
+        <v>0.07822513579003033</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1841531339022194</v>
+        <v>0.02401403681634524</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0005982383516741455</v>
+        <v>8.372401575292929e-05</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01954671242480341</v>
+        <v>0.002660159126982078</v>
       </c>
       <c r="G6" t="n">
-        <v>2.243393818778045e-05</v>
+        <v>3.139650590734848e-06</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0007451094171468894</v>
+        <v>0.000101456224444874</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0001273964138132682</v>
+        <v>1.783003391926049e-05</v>
       </c>
       <c r="J6" t="n">
-        <v>0.004258755709809346</v>
+        <v>0.0005800438410456883</v>
       </c>
       <c r="K6" t="n">
-        <v>5.515205236754834e-05</v>
+        <v>7.864779485592351e-06</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0007290662323813206</v>
+        <v>9.923521352973044e-05</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>1.441573086559354</v>
+        <v>0.2059850558349479</v>
       </c>
     </row>
     <row r="7">
@@ -730,43 +730,43 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3950488935544532</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7903091162295177</v>
+        <v>0.07353162764262851</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2025092421498664</v>
+        <v>0.02510543944129527</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0008024714385099327</v>
+        <v>0.0001101965874914616</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02189480104361739</v>
+        <v>0.002855303942640225</v>
       </c>
       <c r="G7" t="n">
-        <v>3.009267894412248e-05</v>
+        <v>4.132372030929808e-06</v>
       </c>
       <c r="H7" t="n">
-        <v>0.000834857334227037</v>
+        <v>0.0001089507847710486</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0001707883633715627</v>
+        <v>2.345437235768923e-05</v>
       </c>
       <c r="J7" t="n">
-        <v>0.004772875656516981</v>
+        <v>0.000623113635203065</v>
       </c>
       <c r="K7" t="n">
-        <v>7.547587986205919e-05</v>
+        <v>1.070913948689879e-05</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0008167274476885717</v>
+        <v>0.0001065315430307197</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>1.417265341776575</v>
+        <v>0.2026718898037573</v>
       </c>
     </row>
     <row r="8">
@@ -774,43 +774,43 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3292647662262045</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8086746965839954</v>
+        <v>0.0691197299840708</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2195514028011575</v>
+        <v>0.02575152118365869</v>
       </c>
       <c r="E8" t="n">
-        <v>0.001023013328811494</v>
+        <v>0.000137237610371255</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02408144988626477</v>
+        <v>0.00298573292632188</v>
       </c>
       <c r="G8" t="n">
-        <v>3.836299983043104e-05</v>
+        <v>5.14641038892206e-06</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0009183749060616591</v>
+        <v>0.0001139583779355288</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0002176461459453748</v>
+        <v>2.919953698920423e-05</v>
       </c>
       <c r="J8" t="n">
-        <v>0.005251236499678021</v>
+        <v>0.0006519194254799083</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001027353591913873</v>
+        <v>1.445249184493044e-05</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0008983480896995168</v>
+        <v>0.0001114087381127642</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>1.39002203282684</v>
+        <v>0.1991127370279954</v>
       </c>
     </row>
     <row r="9">
@@ -818,43 +818,43 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2697048107417248</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8197141702734354</v>
+        <v>0.06497254618502656</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2351391741760236</v>
+        <v>0.02603597680515414</v>
       </c>
       <c r="E9" t="n">
-        <v>0.001257830638966161</v>
+        <v>0.0001642967827012502</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02611247634064593</v>
+        <v>0.003063274331080456</v>
       </c>
       <c r="G9" t="n">
-        <v>4.716864896123105e-05</v>
+        <v>6.161129351296884e-06</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0009959179726567527</v>
+        <v>0.0001169338194051487</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0002675376615731995</v>
+        <v>3.494858785533948e-05</v>
       </c>
       <c r="J9" t="n">
-        <v>0.00569538614585585</v>
+        <v>0.0006690680075629291</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0001374843512411309</v>
+        <v>1.911414226831253e-05</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0009741542340481884</v>
+        <v>0.0001143089465474045</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>1.360046111185132</v>
+        <v>0.1953890590797743</v>
       </c>
     </row>
     <row r="10">
@@ -862,43 +862,43 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2174595847269764</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8227765460717776</v>
+        <v>0.06107419341392496</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2490511482660261</v>
+        <v>0.02602893305548261</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001504778390086337</v>
+        <v>0.0001909396449518002</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02797113676370552</v>
+        <v>0.003097855080828918</v>
       </c>
       <c r="G10" t="n">
-        <v>5.642918962823764e-05</v>
+        <v>7.160236685692507e-06</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001066865829623726</v>
+        <v>0.0001182587927634216</v>
       </c>
       <c r="I10" t="n">
-        <v>0.000320007096464036</v>
+        <v>4.060920148070428e-05</v>
       </c>
       <c r="J10" t="n">
-        <v>0.006101824188918121</v>
+        <v>0.0006767481134661974</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001802076620112761</v>
+        <v>2.469470792202909e-05</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001043526145171184</v>
+        <v>0.0001156032716841219</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>1.327532054330388</v>
+        <v>0.1915674258620119</v>
       </c>
     </row>
     <row r="11">
@@ -906,43 +906,43 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1728730253175389</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8179965127169085</v>
+        <v>0.05740974180908946</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2610600687904289</v>
+        <v>0.02578904470199572</v>
       </c>
       <c r="E11" t="n">
-        <v>0.001761505973083151</v>
+        <v>0.0002168280545597289</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02963106546515542</v>
+        <v>0.003097793590659432</v>
       </c>
       <c r="G11" t="n">
-        <v>6.605647399061816e-05</v>
+        <v>8.131052045989835e-06</v>
       </c>
       <c r="H11" t="n">
-        <v>0.001130220062619847</v>
+        <v>0.0001182531173417854</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0003745549405708796</v>
+        <v>4.610952176839262e-05</v>
       </c>
       <c r="J11" t="n">
-        <v>0.006464859321873347</v>
+        <v>0.0006767937850875247</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0002313172527893831</v>
+        <v>3.118005148579132e-05</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00110548214486326</v>
+        <v>0.0001156026836192444</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>1.292694668459822</v>
+        <v>0.1877019087104746</v>
       </c>
     </row>
     <row r="12">
@@ -950,43 +950,43 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1357337436702637</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8060560036011692</v>
+        <v>0.0539651573005441</v>
       </c>
       <c r="D12" t="n">
-        <v>0.270980849234879</v>
+        <v>0.02536527250524172</v>
       </c>
       <c r="E12" t="n">
-        <v>0.002025455888385338</v>
+        <v>0.0002417037226744514</v>
       </c>
       <c r="F12" t="n">
-        <v>0.03106519599611967</v>
+        <v>0.003070048206984779</v>
       </c>
       <c r="G12" t="n">
-        <v>7.595459581445016e-05</v>
+        <v>9.063889600291926e-06</v>
       </c>
       <c r="H12" t="n">
-        <v>0.001184948875676186</v>
+        <v>0.0001171843046238216</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0004306377197764544</v>
+        <v>5.139466155788653e-05</v>
       </c>
       <c r="J12" t="n">
-        <v>0.006778588842880892</v>
+        <v>0.0006707391326479288</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0002911452568505292</v>
+        <v>3.854455212700506e-05</v>
       </c>
       <c r="L12" t="n">
-        <v>0.00115901252268354</v>
+        <v>0.0001145673062814577</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>1.255781536204499</v>
+        <v>0.1838361059251049</v>
       </c>
     </row>
     <row r="13">
@@ -994,43 +994,43 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1054532548958411</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7879731321595217</v>
+        <v>0.05072724786251145</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2786970820657173</v>
+        <v>0.02479839106748811</v>
       </c>
       <c r="E13" t="n">
-        <v>0.002293920142592403</v>
+        <v>0.0002653743454458568</v>
       </c>
       <c r="F13" t="n">
-        <v>0.03225146565545564</v>
+        <v>0.003020427951952543</v>
       </c>
       <c r="G13" t="n">
-        <v>8.602200534721511e-05</v>
+        <v>9.951537954219629e-06</v>
       </c>
       <c r="H13" t="n">
-        <v>0.001230207691529504</v>
+        <v>0.000115275664520554</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0004876799801776078</v>
+        <v>5.642375552310235e-05</v>
       </c>
       <c r="J13" t="n">
-        <v>0.007038168474262355</v>
+        <v>0.0006598648131548821</v>
       </c>
       <c r="K13" t="n">
-        <v>0.000359936953357352</v>
+        <v>4.675381737338737e-05</v>
       </c>
       <c r="L13" t="n">
-        <v>0.00120329317772213</v>
+        <v>0.0001127142962436338</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>1.217074163201525</v>
+        <v>0.1800048554549892</v>
       </c>
     </row>
     <row r="14">
@@ -1038,43 +1038,43 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.08122352199166959</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7649244771341219</v>
+        <v>0.04768361299076077</v>
       </c>
       <c r="D14" t="n">
-        <v>0.284170907685431</v>
+        <v>0.02412226727911558</v>
       </c>
       <c r="E14" t="n">
-        <v>0.002564126877078677</v>
+        <v>0.0002877019330543586</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03317596642555665</v>
+        <v>0.002953771252270062</v>
       </c>
       <c r="G14" t="n">
-        <v>9.615475789045036e-05</v>
+        <v>1.078882248953844e-05</v>
       </c>
       <c r="H14" t="n">
-        <v>0.001265461529818443</v>
+        <v>0.0001127131800973583</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0005450926966593927</v>
+        <v>6.116748009066496e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>0.007240518539350068</v>
+        <v>0.0006452374485615445</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0004378456565185131</v>
+        <v>5.576692399716809e-05</v>
       </c>
       <c r="L14" t="n">
-        <v>0.00123780377954357</v>
+        <v>0.0001102245246268954</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>1.176881877073638</v>
+        <v>0.1762356821778855</v>
       </c>
     </row>
     <row r="15">
@@ -1082,43 +1082,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.06214598912384005</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7381065413739042</v>
+        <v>0.04482259621131512</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2874407401606637</v>
+        <v>0.02336494396669389</v>
       </c>
       <c r="E15" t="n">
-        <v>0.002833336413742991</v>
+        <v>0.0003085929996637752</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0338341199251522</v>
+        <v>0.002874097479010813</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0001062501155153621</v>
+        <v>1.157223748739157e-05</v>
       </c>
       <c r="H15" t="n">
-        <v>0.001290531347417073</v>
+        <v>0.0001096513364223486</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0006022936826127146</v>
+        <v>6.560596880430081e-05</v>
       </c>
       <c r="J15" t="n">
-        <v>0.007384593654013793</v>
+        <v>0.0006277430472144137</v>
       </c>
       <c r="K15" t="n">
-        <v>0.000524930546697753</v>
+        <v>6.553826254729987e-05</v>
       </c>
       <c r="L15" t="n">
-        <v>0.001262372034323321</v>
+        <v>0.0001072482425152038</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>1.135531698377883</v>
+        <v>0.172550020094496</v>
       </c>
     </row>
     <row r="16">
@@ -1126,43 +1126,43 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.04732759066751309</v>
+        <v>0.1001924303428215</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7086385473477969</v>
+        <v>0.04213324043863621</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2886110216189984</v>
+        <v>0.02254955814436871</v>
       </c>
       <c r="E16" t="n">
-        <v>0.003098931882350984</v>
+        <v>0.0003279903284332221</v>
       </c>
       <c r="F16" t="n">
-        <v>0.03423041002072676</v>
+        <v>0.00278473539953345</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0001162099455881619</v>
+        <v>1.229963731624583e-05</v>
       </c>
       <c r="H16" t="n">
-        <v>0.001305584805555648</v>
+        <v>0.0001062180612982148</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0006587268482405278</v>
+        <v>6.972706238928733e-05</v>
       </c>
       <c r="J16" t="n">
-        <v>0.007471333160687757</v>
+        <v>0.0006081153331131266</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0006211577632845155</v>
+        <v>7.601904872754684e-05</v>
       </c>
       <c r="L16" t="n">
-        <v>0.001277163991553548</v>
+        <v>0.0001039098832053616</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>1.093356678052296</v>
+        <v>0.1689642436798429</v>
       </c>
     </row>
     <row r="17">
@@ -1170,43 +1170,43 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.03594391918243994</v>
+        <v>0.03658806804351665</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6775039059920022</v>
+        <v>0.1032096083116229</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2878376812170164</v>
+        <v>0.02169511884903157</v>
       </c>
       <c r="E17" t="n">
-        <v>0.003358495015587955</v>
+        <v>0.0003458660690103344</v>
       </c>
       <c r="F17" t="n">
-        <v>0.03437716828611342</v>
+        <v>0.002688432026108409</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0001259435630845483</v>
+        <v>1.296997758788754e-05</v>
       </c>
       <c r="H17" t="n">
-        <v>0.001311090446540417</v>
+        <v>0.000102518911922348</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0007138783070026377</v>
+        <v>7.352484196920131e-05</v>
       </c>
       <c r="J17" t="n">
-        <v>0.007503401035747628</v>
+        <v>0.0005869597515481801</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0007264045753143201</v>
+        <v>8.715855511024398e-05</v>
       </c>
       <c r="L17" t="n">
-        <v>0.00128263888858664</v>
+        <v>0.0001003121315681446</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>1.050684526509436</v>
+        <v>0.1654905374689959</v>
       </c>
     </row>
     <row r="18">
@@ -1214,43 +1214,43 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.02727379174787814</v>
+        <v>0.01418469763434395</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6455237990670438</v>
+        <v>0.1194204022220982</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2853122633939841</v>
+        <v>0.02463342752037421</v>
       </c>
       <c r="E18" t="n">
-        <v>0.003609862372611912</v>
+        <v>0.0003622159616968829</v>
       </c>
       <c r="F18" t="n">
-        <v>0.03429284873353516</v>
+        <v>0.002587444821873152</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0001353698389729467</v>
+        <v>1.358309856363311e-05</v>
       </c>
       <c r="H18" t="n">
-        <v>0.001307752024484692</v>
+        <v>9.86406213637292e-05</v>
       </c>
       <c r="I18" t="n">
-        <v>0.000767288323116903</v>
+        <v>7.699840170056671e-05</v>
       </c>
       <c r="J18" t="n">
-        <v>0.007484811232463836</v>
+        <v>0.000564773804113854</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0008404661261269205</v>
+        <v>9.890510843745981e-05</v>
       </c>
       <c r="L18" t="n">
-        <v>0.001279484839469663</v>
+        <v>9.653937120688473e-05</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>1.007827737699688</v>
+        <v>0.1621376285657725</v>
       </c>
     </row>
     <row r="19">
@@ -1258,43 +1258,43 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.02071178317371192</v>
+        <v>0.005222413989233897</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6133543796971874</v>
+        <v>0.1212174617338824</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2812468518289091</v>
+        <v>0.02810363752564397</v>
       </c>
       <c r="E19" t="n">
-        <v>0.003851160942251559</v>
+        <v>0.0003816340277938192</v>
       </c>
       <c r="F19" t="n">
-        <v>0.03400014388624832</v>
+        <v>0.002936991673905836</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0001444185353344334</v>
+        <v>1.431127604226822e-05</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001296436522695202</v>
+        <v>0.0001116555476577235</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0008185588772350957</v>
+        <v>8.112397047064627e-05</v>
       </c>
       <c r="J19" t="n">
-        <v>0.007420516096245826</v>
+        <v>0.0006383057954515601</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0009630640874043328</v>
+        <v>0.0001112068907719206</v>
       </c>
       <c r="L19" t="n">
-        <v>0.001268548529928728</v>
+        <v>0.0001094920350338763</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>0.9650758621771519</v>
+        <v>0.1589282344658879</v>
       </c>
     </row>
     <row r="20">
@@ -1302,43 +1302,43 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.01576579506419083</v>
+        <v>0.001777182209405854</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5814991050248772</v>
+        <v>0.1173896458096775</v>
       </c>
       <c r="D20" t="n">
-        <v>0.275861086836404</v>
+        <v>0.03116113960083032</v>
       </c>
       <c r="E20" t="n">
-        <v>0.004080824658063207</v>
+        <v>0.000404672640046365</v>
       </c>
       <c r="F20" t="n">
-        <v>0.03352419478069391</v>
+        <v>0.003349817688255304</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0001530309246773702</v>
+        <v>1.517522400173869e-05</v>
       </c>
       <c r="H20" t="n">
-        <v>0.001278105593438077</v>
+        <v>0.0001273678228013037</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0008673571758888849</v>
+        <v>8.601892686650739e-05</v>
       </c>
       <c r="J20" t="n">
-        <v>0.007316013792821563</v>
+        <v>0.0007280510279825225</v>
       </c>
       <c r="K20" t="n">
-        <v>0.001093856522311167</v>
+        <v>0.0001241680994193833</v>
       </c>
       <c r="L20" t="n">
-        <v>0.001250768369074226</v>
+        <v>0.0001248834179431609</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9226901387424405</v>
+        <v>0.15528812246723</v>
       </c>
     </row>
     <row r="21">
@@ -1346,43 +1346,43 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.01204590676195057</v>
+        <v>0.0005586466071316881</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5503290470256248</v>
+        <v>0.111564802663371</v>
       </c>
       <c r="D21" t="n">
-        <v>0.269371870112436</v>
+        <v>0.03353034740928642</v>
       </c>
       <c r="E21" t="n">
-        <v>0.004297594871841122</v>
+        <v>0.0004307351736460632</v>
       </c>
       <c r="F21" t="n">
-        <v>0.03289104911371443</v>
+        <v>0.003713719358403991</v>
       </c>
       <c r="G21" t="n">
-        <v>0.000161159807694042</v>
+        <v>1.615256901172737e-05</v>
       </c>
       <c r="H21" t="n">
-        <v>0.001253756390368878</v>
+        <v>0.0001412938126840444</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0009134157521072791</v>
+        <v>9.155648751245692e-05</v>
       </c>
       <c r="J21" t="n">
-        <v>0.007177009138556126</v>
+        <v>0.0008078492541372528</v>
       </c>
       <c r="K21" t="n">
-        <v>0.001232448309494453</v>
+        <v>0.0001379116905233447</v>
       </c>
       <c r="L21" t="n">
-        <v>0.001227116875375494</v>
+        <v>0.0001384729346299182</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>0.8809003741591631</v>
+        <v>0.1511314879603379</v>
       </c>
     </row>
     <row r="22">
@@ -1390,43 +1390,43 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00924928192884648</v>
+        <v>0.0001640771271126538</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5201059290371914</v>
+        <v>0.1052654839835878</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2619858324171081</v>
+        <v>0.03519468345769572</v>
       </c>
       <c r="E22" t="n">
-        <v>0.004500508459564494</v>
+        <v>0.0004589110056751172</v>
       </c>
       <c r="F22" t="n">
-        <v>0.03212643818012798</v>
+        <v>0.003995939665776327</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0001687690672336685</v>
+        <v>1.720916271281689e-05</v>
       </c>
       <c r="H22" t="n">
-        <v>0.001224374555324059</v>
+        <v>0.0001521187976744415</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0009565299379269465</v>
+        <v>9.754314445147617e-05</v>
       </c>
       <c r="J22" t="n">
-        <v>0.007009143826920431</v>
+        <v>0.0008699820336428298</v>
       </c>
       <c r="K22" t="n">
-        <v>0.001378401583164016</v>
+        <v>0.0001525403585340919</v>
       </c>
       <c r="L22" t="n">
-        <v>0.001198554951317933</v>
+        <v>0.0001490200269360635</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>0.8399037639447255</v>
+        <v>0.1465175087637993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>